<commit_message>
Pushing UI and API to Git
</commit_message>
<xml_diff>
--- a/CrudeOilDemandCode/RefDocs/Output.xlsx
+++ b/CrudeOilDemandCode/RefDocs/Output.xlsx
@@ -460,7 +460,7 @@
         <v>2023</v>
       </c>
       <c r="C2" t="n">
-        <v>2379.404606934405</v>
+        <v>2375.553533848452</v>
       </c>
     </row>
     <row r="3">
@@ -473,7 +473,7 @@
         <v>2024</v>
       </c>
       <c r="C3" t="n">
-        <v>2347.460628792699</v>
+        <v>2343.776963035138</v>
       </c>
     </row>
     <row r="4">
@@ -486,7 +486,7 @@
         <v>2025</v>
       </c>
       <c r="C4" t="n">
-        <v>2379.404606934405</v>
+        <v>2375.553533848452</v>
       </c>
     </row>
     <row r="5">
@@ -499,7 +499,7 @@
         <v>2026</v>
       </c>
       <c r="C5" t="n">
-        <v>2379.404606934405</v>
+        <v>2375.553533848452</v>
       </c>
     </row>
     <row r="6">
@@ -512,7 +512,7 @@
         <v>2027</v>
       </c>
       <c r="C6" t="n">
-        <v>2348.170873735071</v>
+        <v>2348.940742550856</v>
       </c>
     </row>
     <row r="7">
@@ -525,7 +525,7 @@
         <v>2028</v>
       </c>
       <c r="C7" t="n">
-        <v>2348.170873735071</v>
+        <v>2348.940742550856</v>
       </c>
     </row>
     <row r="8">
@@ -538,7 +538,7 @@
         <v>2023</v>
       </c>
       <c r="C8" t="n">
-        <v>2042.233618668764</v>
+        <v>2042.996992853785</v>
       </c>
     </row>
     <row r="9">
@@ -551,7 +551,7 @@
         <v>2024</v>
       </c>
       <c r="C9" t="n">
-        <v>2061.684687745817</v>
+        <v>2054.322229650993</v>
       </c>
     </row>
     <row r="10">
@@ -564,7 +564,7 @@
         <v>2025</v>
       </c>
       <c r="C10" t="n">
-        <v>2028.611430348353</v>
+        <v>2029.362860345671</v>
       </c>
     </row>
     <row r="11">
@@ -577,7 +577,7 @@
         <v>2026</v>
       </c>
       <c r="C11" t="n">
-        <v>1958.206442444451</v>
+        <v>2039.511913560559</v>
       </c>
     </row>
     <row r="12">
@@ -590,7 +590,7 @@
         <v>2027</v>
       </c>
       <c r="C12" t="n">
-        <v>1982.735243940004</v>
+        <v>1978.054592518947</v>
       </c>
     </row>
     <row r="13">
@@ -603,7 +603,7 @@
         <v>2028</v>
       </c>
       <c r="C13" t="n">
-        <v>1955.4532453301</v>
+        <v>1942.811553016351</v>
       </c>
     </row>
     <row r="14">
@@ -616,7 +616,7 @@
         <v>2023</v>
       </c>
       <c r="C14" t="n">
-        <v>20171.14360308905</v>
+        <v>20060.98989507073</v>
       </c>
     </row>
     <row r="15">
@@ -629,7 +629,7 @@
         <v>2024</v>
       </c>
       <c r="C15" t="n">
-        <v>20358.30439889022</v>
+        <v>20172.47624064033</v>
       </c>
     </row>
     <row r="16">
@@ -642,7 +642,7 @@
         <v>2025</v>
       </c>
       <c r="C16" t="n">
-        <v>20249.73851722959</v>
+        <v>20172.47624064033</v>
       </c>
     </row>
     <row r="17">
@@ -655,7 +655,7 @@
         <v>2026</v>
       </c>
       <c r="C17" t="n">
-        <v>19592.69184340419</v>
+        <v>19663.49715172883</v>
       </c>
     </row>
     <row r="18">
@@ -668,7 +668,7 @@
         <v>2027</v>
       </c>
       <c r="C18" t="n">
-        <v>20159.87307335501</v>
+        <v>20252.92847467912</v>
       </c>
     </row>
     <row r="19">
@@ -681,7 +681,7 @@
         <v>2028</v>
       </c>
       <c r="C19" t="n">
-        <v>20335.25611678885</v>
+        <v>20442.06886548464</v>
       </c>
     </row>
     <row r="20">
@@ -694,7 +694,7 @@
         <v>2023</v>
       </c>
       <c r="C20" t="n">
-        <v>1536.98209424635</v>
+        <v>1556.628165139704</v>
       </c>
     </row>
     <row r="21">
@@ -707,7 +707,7 @@
         <v>2024</v>
       </c>
       <c r="C21" t="n">
-        <v>1536.98209424635</v>
+        <v>1556.628165139704</v>
       </c>
     </row>
     <row r="22">
@@ -720,7 +720,7 @@
         <v>2025</v>
       </c>
       <c r="C22" t="n">
-        <v>1489.508485787259</v>
+        <v>1497.392386900223</v>
       </c>
     </row>
     <row r="23">
@@ -733,7 +733,7 @@
         <v>2026</v>
       </c>
       <c r="C23" t="n">
-        <v>1422.583045712414</v>
+        <v>1433.340338412169</v>
       </c>
     </row>
     <row r="24">
@@ -746,7 +746,7 @@
         <v>2027</v>
       </c>
       <c r="C24" t="n">
-        <v>1386.307091798032</v>
+        <v>1400.948862870578</v>
       </c>
     </row>
     <row r="25">
@@ -759,7 +759,7 @@
         <v>2028</v>
       </c>
       <c r="C25" t="n">
-        <v>1450.350019178073</v>
+        <v>1456.875815862063</v>
       </c>
     </row>
     <row r="26">
@@ -772,7 +772,7 @@
         <v>2023</v>
       </c>
       <c r="C26" t="n">
-        <v>2477.442087884534</v>
+        <v>2472.622910278986</v>
       </c>
     </row>
     <row r="27">
@@ -785,7 +785,7 @@
         <v>2024</v>
       </c>
       <c r="C27" t="n">
-        <v>2228.818331473126</v>
+        <v>2223.999680159021</v>
       </c>
     </row>
     <row r="28">
@@ -798,7 +798,7 @@
         <v>2025</v>
       </c>
       <c r="C28" t="n">
-        <v>2237.975490980428</v>
+        <v>2223.999680159021</v>
       </c>
     </row>
     <row r="29">
@@ -811,7 +811,7 @@
         <v>2026</v>
       </c>
       <c r="C29" t="n">
-        <v>2213.939055722316</v>
+        <v>2192.917481138555</v>
       </c>
     </row>
     <row r="30">
@@ -824,7 +824,7 @@
         <v>2027</v>
       </c>
       <c r="C30" t="n">
-        <v>2183.429237318876</v>
+        <v>2170.395154017165</v>
       </c>
     </row>
     <row r="31">
@@ -837,7 +837,7 @@
         <v>2028</v>
       </c>
       <c r="C31" t="n">
-        <v>2197.963826838119</v>
+        <v>2180.639637307194</v>
       </c>
     </row>
     <row r="32">
@@ -850,7 +850,7 @@
         <v>2023</v>
       </c>
       <c r="C32" t="n">
-        <v>1270.583700842307</v>
+        <v>1269.752317301101</v>
       </c>
     </row>
     <row r="33">
@@ -863,7 +863,7 @@
         <v>2024</v>
       </c>
       <c r="C33" t="n">
-        <v>1265.50767692952</v>
+        <v>1264.57568970012</v>
       </c>
     </row>
     <row r="34">
@@ -876,7 +876,7 @@
         <v>2025</v>
       </c>
       <c r="C34" t="n">
-        <v>1261.87955086211</v>
+        <v>1264.57568970012</v>
       </c>
     </row>
     <row r="35">
@@ -889,7 +889,7 @@
         <v>2026</v>
       </c>
       <c r="C35" t="n">
-        <v>1183.126672144555</v>
+        <v>1179.823258639975</v>
       </c>
     </row>
     <row r="36">
@@ -902,7 +902,7 @@
         <v>2027</v>
       </c>
       <c r="C36" t="n">
-        <v>1230.752134422893</v>
+        <v>1226.182278134155</v>
       </c>
     </row>
     <row r="37">
@@ -915,7 +915,7 @@
         <v>2028</v>
       </c>
       <c r="C37" t="n">
-        <v>1230.621500425131</v>
+        <v>1212.954307496976</v>
       </c>
     </row>
     <row r="38">
@@ -928,7 +928,7 @@
         <v>2023</v>
       </c>
       <c r="C38" t="n">
-        <v>1195.415990893331</v>
+        <v>1195.469426699615</v>
       </c>
     </row>
     <row r="39">
@@ -941,7 +941,7 @@
         <v>2024</v>
       </c>
       <c r="C39" t="n">
-        <v>1159.454308118194</v>
+        <v>1149.435295122411</v>
       </c>
     </row>
     <row r="40">
@@ -954,7 +954,7 @@
         <v>2025</v>
       </c>
       <c r="C40" t="n">
-        <v>1182.664342425552</v>
+        <v>1164.417946995289</v>
       </c>
     </row>
     <row r="41">
@@ -967,7 +967,7 @@
         <v>2026</v>
       </c>
       <c r="C41" t="n">
-        <v>1134.247520484838</v>
+        <v>1121.200725318295</v>
       </c>
     </row>
     <row r="42">
@@ -980,7 +980,7 @@
         <v>2027</v>
       </c>
       <c r="C42" t="n">
-        <v>1138.860872914305</v>
+        <v>1121.341595103268</v>
       </c>
     </row>
     <row r="43">
@@ -993,7 +993,7 @@
         <v>2028</v>
       </c>
       <c r="C43" t="n">
-        <v>1143.218620624759</v>
+        <v>1125.444185667789</v>
       </c>
     </row>
     <row r="44">
@@ -1006,7 +1006,7 @@
         <v>2023</v>
       </c>
       <c r="C44" t="n">
-        <v>922.0003631989016</v>
+        <v>921.1366307298617</v>
       </c>
     </row>
     <row r="45">
@@ -1019,7 +1019,7 @@
         <v>2024</v>
       </c>
       <c r="C45" t="n">
-        <v>937.5667998648258</v>
+        <v>921.1366307298617</v>
       </c>
     </row>
     <row r="46">
@@ -1032,7 +1032,7 @@
         <v>2025</v>
       </c>
       <c r="C46" t="n">
-        <v>918.3722371314917</v>
+        <v>921.1366307298617</v>
       </c>
     </row>
     <row r="47">
@@ -1045,7 +1045,7 @@
         <v>2026</v>
       </c>
       <c r="C47" t="n">
-        <v>899.9680445667149</v>
+        <v>899.664551057899</v>
       </c>
     </row>
     <row r="48">
@@ -1058,7 +1058,7 @@
         <v>2027</v>
       </c>
       <c r="C48" t="n">
-        <v>948.8304204425668</v>
+        <v>942.9843646082304</v>
       </c>
     </row>
     <row r="49">
@@ -1071,7 +1071,7 @@
         <v>2028</v>
       </c>
       <c r="C49" t="n">
-        <v>948.8304204425668</v>
+        <v>942.9843646082304</v>
       </c>
     </row>
     <row r="50">
@@ -1084,7 +1084,7 @@
         <v>2023</v>
       </c>
       <c r="C50" t="n">
-        <v>1326.240857370182</v>
+        <v>1326.104443508854</v>
       </c>
     </row>
     <row r="51">
@@ -1097,7 +1097,7 @@
         <v>2024</v>
       </c>
       <c r="C51" t="n">
-        <v>1326.240857370182</v>
+        <v>1326.104443508854</v>
       </c>
     </row>
     <row r="52">
@@ -1110,7 +1110,7 @@
         <v>2025</v>
       </c>
       <c r="C52" t="n">
-        <v>1304.153223826592</v>
+        <v>1310.176744372151</v>
       </c>
     </row>
     <row r="53">
@@ -1123,7 +1123,7 @@
         <v>2026</v>
       </c>
       <c r="C53" t="n">
-        <v>1291.727541823457</v>
+        <v>1304.174808347777</v>
       </c>
     </row>
     <row r="54">
@@ -1136,7 +1136,7 @@
         <v>2027</v>
       </c>
       <c r="C54" t="n">
-        <v>1258.298632664992</v>
+        <v>1274.393002091884</v>
       </c>
     </row>
     <row r="55">
@@ -1149,7 +1149,7 @@
         <v>2028</v>
       </c>
       <c r="C55" t="n">
-        <v>1269.397768524771</v>
+        <v>1278.495592656406</v>
       </c>
     </row>
     <row r="56">
@@ -1162,7 +1162,7 @@
         <v>2023</v>
       </c>
       <c r="C56" t="n">
-        <v>1109.965789273129</v>
+        <v>1110.533486579043</v>
       </c>
     </row>
     <row r="57">
@@ -1175,7 +1175,7 @@
         <v>2024</v>
       </c>
       <c r="C57" t="n">
-        <v>1057.677316938988</v>
+        <v>1055.029172650482</v>
       </c>
     </row>
     <row r="58">
@@ -1188,7 +1188,7 @@
         <v>2025</v>
       </c>
       <c r="C58" t="n">
-        <v>1189.77238055292</v>
+        <v>1185.823539096346</v>
       </c>
     </row>
     <row r="59">
@@ -1201,7 +1201,7 @@
         <v>2026</v>
       </c>
       <c r="C59" t="n">
-        <v>1170.617337227105</v>
+        <v>1166.590835918455</v>
       </c>
     </row>
     <row r="60">
@@ -1214,7 +1214,7 @@
         <v>2027</v>
       </c>
       <c r="C60" t="n">
-        <v>1170.617337227105</v>
+        <v>1166.590835918455</v>
       </c>
     </row>
     <row r="61">
@@ -1227,7 +1227,7 @@
         <v>2028</v>
       </c>
       <c r="C61" t="n">
-        <v>1174.975084937558</v>
+        <v>1170.693426482977</v>
       </c>
     </row>
     <row r="62">
@@ -1240,7 +1240,7 @@
         <v>2023</v>
       </c>
       <c r="C62" t="n">
-        <v>1557.872951427203</v>
+        <v>1549.711507040808</v>
       </c>
     </row>
     <row r="63">
@@ -1253,7 +1253,7 @@
         <v>2024</v>
       </c>
       <c r="C63" t="n">
-        <v>1627.557830485599</v>
+        <v>1625.096184762227</v>
       </c>
     </row>
     <row r="64">
@@ -1266,7 +1266,7 @@
         <v>2025</v>
       </c>
       <c r="C64" t="n">
-        <v>1627.557830485599</v>
+        <v>1625.096184762227</v>
       </c>
     </row>
     <row r="65">
@@ -1279,7 +1279,7 @@
         <v>2026</v>
       </c>
       <c r="C65" t="n">
-        <v>1454.462381939975</v>
+        <v>1444.442677860478</v>
       </c>
     </row>
     <row r="66">
@@ -1292,7 +1292,7 @@
         <v>2027</v>
       </c>
       <c r="C66" t="n">
-        <v>1363.873509036102</v>
+        <v>1348.542213620639</v>
       </c>
     </row>
     <row r="67">
@@ -1305,7 +1305,7 @@
         <v>2028</v>
       </c>
       <c r="C67" t="n">
-        <v>1346.068428328792</v>
+        <v>1326.971640725344</v>
       </c>
     </row>
     <row r="68">
@@ -1318,7 +1318,7 @@
         <v>2023</v>
       </c>
       <c r="C68" t="n">
-        <v>1137.105019064915</v>
+        <v>1128.813106177955</v>
       </c>
     </row>
     <row r="69">
@@ -1331,7 +1331,7 @@
         <v>2024</v>
       </c>
       <c r="C69" t="n">
-        <v>1132.162225244659</v>
+        <v>1125.374733954056</v>
       </c>
     </row>
     <row r="70">
@@ -1344,7 +1344,7 @@
         <v>2025</v>
       </c>
       <c r="C70" t="n">
-        <v>1107.842295571048</v>
+        <v>1102.20540222471</v>
       </c>
     </row>
     <row r="71">
@@ -1357,7 +1357,7 @@
         <v>2026</v>
       </c>
       <c r="C71" t="n">
-        <v>1126.567492107157</v>
+        <v>1125.374733954056</v>
       </c>
     </row>
     <row r="72">
@@ -1370,7 +1370,7 @@
         <v>2027</v>
       </c>
       <c r="C72" t="n">
-        <v>1047.109552810572</v>
+        <v>1048.742565567924</v>
       </c>
     </row>
     <row r="73">
@@ -1383,7 +1383,7 @@
         <v>2028</v>
       </c>
       <c r="C73" t="n">
-        <v>1047.109552810572</v>
+        <v>1048.742565567924</v>
       </c>
     </row>
     <row r="74">
@@ -1396,7 +1396,7 @@
         <v>2023</v>
       </c>
       <c r="C74" t="n">
-        <v>4008.007389610524</v>
+        <v>4008.622999057393</v>
       </c>
     </row>
     <row r="75">
@@ -1409,7 +1409,7 @@
         <v>2024</v>
       </c>
       <c r="C75" t="n">
-        <v>3575.672885064074</v>
+        <v>3586.323824722017</v>
       </c>
     </row>
     <row r="76">
@@ -1422,7 +1422,7 @@
         <v>2025</v>
       </c>
       <c r="C76" t="n">
-        <v>3890.226475864574</v>
+        <v>3879.233787054284</v>
       </c>
     </row>
     <row r="77">
@@ -1435,7 +1435,7 @@
         <v>2026</v>
       </c>
       <c r="C77" t="n">
-        <v>3168.145096763264</v>
+        <v>3168.300350252005</v>
       </c>
     </row>
     <row r="78">
@@ -1448,7 +1448,7 @@
         <v>2027</v>
       </c>
       <c r="C78" t="n">
-        <v>3186.344441602475</v>
+        <v>3193.629945289124</v>
       </c>
     </row>
     <row r="79">
@@ -1461,7 +1461,7 @@
         <v>2028</v>
       </c>
       <c r="C79" t="n">
-        <v>3467.770842981995</v>
+        <v>3463.454956561318</v>
       </c>
     </row>
     <row r="80">
@@ -1474,7 +1474,7 @@
         <v>2023</v>
       </c>
       <c r="C80" t="n">
-        <v>266.5939456733234</v>
+        <v>265.2727661758688</v>
       </c>
     </row>
     <row r="81">
@@ -1487,7 +1487,7 @@
         <v>2024</v>
       </c>
       <c r="C81" t="n">
-        <v>236.9361878694595</v>
+        <v>237.0015010780877</v>
       </c>
     </row>
     <row r="82">
@@ -1500,7 +1500,7 @@
         <v>2025</v>
       </c>
       <c r="C82" t="n">
-        <v>354.3737182511586</v>
+        <v>353.0525387537038</v>
       </c>
     </row>
     <row r="83">
@@ -1513,7 +1513,7 @@
         <v>2026</v>
       </c>
       <c r="C83" t="n">
-        <v>354.3737182511586</v>
+        <v>353.0525387537038</v>
       </c>
     </row>
     <row r="84">
@@ -1526,7 +1526,7 @@
         <v>2027</v>
       </c>
       <c r="C84" t="n">
-        <v>324.2218472515746</v>
+        <v>328.5000562691307</v>
       </c>
     </row>
     <row r="85">
@@ -1539,7 +1539,7 @@
         <v>2028</v>
       </c>
       <c r="C85" t="n">
-        <v>324.2218472515746</v>
+        <v>328.5000562691307</v>
       </c>
     </row>
     <row r="86">
@@ -1552,7 +1552,7 @@
         <v>2023</v>
       </c>
       <c r="C86" t="n">
-        <v>3018.958106067563</v>
+        <v>2679.102706171934</v>
       </c>
     </row>
     <row r="87">
@@ -1565,7 +1565,7 @@
         <v>2024</v>
       </c>
       <c r="C87" t="n">
-        <v>3057.738294788945</v>
+        <v>2733.933373082208</v>
       </c>
     </row>
     <row r="88">
@@ -1578,7 +1578,7 @@
         <v>2025</v>
       </c>
       <c r="C88" t="n">
-        <v>2923.076711488765</v>
+        <v>2910.05686265333</v>
       </c>
     </row>
     <row r="89">
@@ -1591,7 +1591,7 @@
         <v>2026</v>
       </c>
       <c r="C89" t="n">
-        <v>2798.655048992245</v>
+        <v>2791.22993329431</v>
       </c>
     </row>
     <row r="90">
@@ -1604,7 +1604,7 @@
         <v>2027</v>
       </c>
       <c r="C90" t="n">
-        <v>2831.946044189628</v>
+        <v>2829.011456282065</v>
       </c>
     </row>
     <row r="91">
@@ -1617,7 +1617,7 @@
         <v>2028</v>
       </c>
       <c r="C91" t="n">
-        <v>2894.067476802803</v>
+        <v>2892.639761637603</v>
       </c>
     </row>
     <row r="92">
@@ -1630,7 +1630,7 @@
         <v>2023</v>
       </c>
       <c r="C92" t="n">
-        <v>13874.73063936166</v>
+        <v>13871.39536009172</v>
       </c>
     </row>
     <row r="93">
@@ -1643,7 +1643,7 @@
         <v>2024</v>
       </c>
       <c r="C93" t="n">
-        <v>14237.4563616546</v>
+        <v>14275.03494417892</v>
       </c>
     </row>
     <row r="94">
@@ -1656,7 +1656,7 @@
         <v>2025</v>
       </c>
       <c r="C94" t="n">
-        <v>14075.81356596169</v>
+        <v>14168.98056215686</v>
       </c>
     </row>
     <row r="95">
@@ -1669,7 +1669,7 @@
         <v>2026</v>
       </c>
       <c r="C95" t="n">
-        <v>14098.3960796861</v>
+        <v>14179.64168570854</v>
       </c>
     </row>
     <row r="96">
@@ -1682,7 +1682,7 @@
         <v>2027</v>
       </c>
       <c r="C96" t="n">
-        <v>14330.64550569245</v>
+        <v>14391.8918163149</v>
       </c>
     </row>
     <row r="97">
@@ -1695,7 +1695,7 @@
         <v>2028</v>
       </c>
       <c r="C97" t="n">
-        <v>14189.13129466885</v>
+        <v>14281.73484372832</v>
       </c>
     </row>
     <row r="98">
@@ -1708,7 +1708,7 @@
         <v>2023</v>
       </c>
       <c r="C98" t="n">
-        <v>4911.126536159707</v>
+        <v>5227.908173271192</v>
       </c>
     </row>
     <row r="99">
@@ -1721,7 +1721,7 @@
         <v>2024</v>
       </c>
       <c r="C99" t="n">
-        <v>5237.632100639677</v>
+        <v>5227.908173271192</v>
       </c>
     </row>
     <row r="100">
@@ -1734,7 +1734,7 @@
         <v>2025</v>
       </c>
       <c r="C100" t="n">
-        <v>5237.632100639677</v>
+        <v>5227.908173271192</v>
       </c>
     </row>
     <row r="101">
@@ -1747,7 +1747,7 @@
         <v>2026</v>
       </c>
       <c r="C101" t="n">
-        <v>4901.529894012075</v>
+        <v>5215.309203997353</v>
       </c>
     </row>
     <row r="102">
@@ -1760,7 +1760,7 @@
         <v>2027</v>
       </c>
       <c r="C102" t="n">
-        <v>5191.855204369702</v>
+        <v>5187.930582265887</v>
       </c>
     </row>
     <row r="103">
@@ -1773,7 +1773,7 @@
         <v>2028</v>
       </c>
       <c r="C103" t="n">
-        <v>5191.855204369702</v>
+        <v>5190.885592995852</v>
       </c>
     </row>
     <row r="104">
@@ -1786,7 +1786,7 @@
         <v>2023</v>
       </c>
       <c r="C104" t="n">
-        <v>901.8554765331869</v>
+        <v>907.7141737027347</v>
       </c>
     </row>
     <row r="105">
@@ -1799,7 +1799,7 @@
         <v>2024</v>
       </c>
       <c r="C105" t="n">
-        <v>816.2122498319535</v>
+        <v>822.0709476746173</v>
       </c>
     </row>
     <row r="106">
@@ -1812,7 +1812,7 @@
         <v>2025</v>
       </c>
       <c r="C106" t="n">
-        <v>816.2122498319535</v>
+        <v>822.0709476746173</v>
       </c>
     </row>
     <row r="107">
@@ -1825,7 +1825,7 @@
         <v>2026</v>
       </c>
       <c r="C107" t="n">
-        <v>816.2122498319535</v>
+        <v>822.0709476746173</v>
       </c>
     </row>
     <row r="108">
@@ -1838,7 +1838,7 @@
         <v>2027</v>
       </c>
       <c r="C108" t="n">
-        <v>816.2122498319535</v>
+        <v>822.0709476746173</v>
       </c>
     </row>
     <row r="109">
@@ -1851,7 +1851,7 @@
         <v>2028</v>
       </c>
       <c r="C109" t="n">
-        <v>816.2122498319535</v>
+        <v>822.0709476746173</v>
       </c>
     </row>
     <row r="110">
@@ -1864,7 +1864,7 @@
         <v>2023</v>
       </c>
       <c r="C110" t="n">
-        <v>434.2700927300924</v>
+        <v>426.484944206429</v>
       </c>
     </row>
     <row r="111">
@@ -1877,7 +1877,7 @@
         <v>2024</v>
       </c>
       <c r="C111" t="n">
-        <v>434.2700927300924</v>
+        <v>426.484944206429</v>
       </c>
     </row>
     <row r="112">
@@ -1890,7 +1890,7 @@
         <v>2025</v>
       </c>
       <c r="C112" t="n">
-        <v>434.2700927300924</v>
+        <v>426.484944206429</v>
       </c>
     </row>
     <row r="113">
@@ -1903,7 +1903,7 @@
         <v>2026</v>
       </c>
       <c r="C113" t="n">
-        <v>421.1530709529328</v>
+        <v>419.1502344715777</v>
       </c>
     </row>
     <row r="114">
@@ -1916,7 +1916,7 @@
         <v>2027</v>
       </c>
       <c r="C114" t="n">
-        <v>406.0842773152199</v>
+        <v>404.0814408338649</v>
       </c>
     </row>
     <row r="115">
@@ -1929,7 +1929,7 @@
         <v>2028</v>
       </c>
       <c r="C115" t="n">
-        <v>421.1530709529328</v>
+        <v>419.1502344715777</v>
       </c>
     </row>
     <row r="116">
@@ -1942,7 +1942,7 @@
         <v>2023</v>
       </c>
       <c r="C116" t="n">
-        <v>349.4319815189576</v>
+        <v>348.9146051669941</v>
       </c>
     </row>
     <row r="117">
@@ -1955,7 +1955,7 @@
         <v>2024</v>
       </c>
       <c r="C117" t="n">
-        <v>353.3961678202402</v>
+        <v>350.9610384721077</v>
       </c>
     </row>
     <row r="118">
@@ -1968,7 +1968,7 @@
         <v>2025</v>
       </c>
       <c r="C118" t="n">
-        <v>386.3446909582127</v>
+        <v>383.9095616100801</v>
       </c>
     </row>
     <row r="119">
@@ -1981,7 +1981,7 @@
         <v>2026</v>
       </c>
       <c r="C119" t="n">
-        <v>386.3446909582127</v>
+        <v>383.9095616100801</v>
       </c>
     </row>
     <row r="120">
@@ -1994,7 +1994,7 @@
         <v>2027</v>
       </c>
       <c r="C120" t="n">
-        <v>412.0382624607938</v>
+        <v>411.5208861088303</v>
       </c>
     </row>
     <row r="121">
@@ -2007,7 +2007,7 @@
         <v>2028</v>
       </c>
       <c r="C121" t="n">
-        <v>543.9246324459981</v>
+        <v>538.8805350539859</v>
       </c>
     </row>
     <row r="122">
@@ -2020,7 +2020,7 @@
         <v>2023</v>
       </c>
       <c r="C122" t="n">
-        <v>2704.348639636956</v>
+        <v>2716.030410733037</v>
       </c>
     </row>
     <row r="123">
@@ -2033,7 +2033,7 @@
         <v>2024</v>
       </c>
       <c r="C123" t="n">
-        <v>2804.591535879234</v>
+        <v>2805.990132450204</v>
       </c>
     </row>
     <row r="124">
@@ -2046,7 +2046,7 @@
         <v>2025</v>
       </c>
       <c r="C124" t="n">
-        <v>2771.574694537505</v>
+        <v>2772.803572747229</v>
       </c>
     </row>
     <row r="125">
@@ -2059,7 +2059,7 @@
         <v>2026</v>
       </c>
       <c r="C125" t="n">
-        <v>2654.850763052747</v>
+        <v>2657.335120812977</v>
       </c>
     </row>
     <row r="126">
@@ -2072,7 +2072,7 @@
         <v>2027</v>
       </c>
       <c r="C126" t="n">
-        <v>2654.850763052747</v>
+        <v>2657.335120812977</v>
       </c>
     </row>
     <row r="127">
@@ -2085,7 +2085,7 @@
         <v>2028</v>
       </c>
       <c r="C127" t="n">
-        <v>2804.771420492724</v>
+        <v>2810.719920762579</v>
       </c>
     </row>
     <row r="128">
@@ -2098,7 +2098,7 @@
         <v>2023</v>
       </c>
       <c r="C128" t="n">
-        <v>161.2857748753872</v>
+        <v>158.3982980600248</v>
       </c>
     </row>
     <row r="129">
@@ -2111,7 +2111,7 @@
         <v>2024</v>
       </c>
       <c r="C129" t="n">
-        <v>157.0412687264329</v>
+        <v>151.9805821906199</v>
       </c>
     </row>
     <row r="130">
@@ -2124,7 +2124,7 @@
         <v>2025</v>
       </c>
       <c r="C130" t="n">
-        <v>156.6893560179807</v>
+        <v>153.8823344314395</v>
       </c>
     </row>
     <row r="131">
@@ -2137,7 +2137,7 @@
         <v>2026</v>
       </c>
       <c r="C131" t="n">
-        <v>160.535634258437</v>
+        <v>153.4672872230555</v>
       </c>
     </row>
     <row r="132">
@@ -2150,7 +2150,7 @@
         <v>2027</v>
       </c>
       <c r="C132" t="n">
-        <v>157.0412687264329</v>
+        <v>151.9805821906199</v>
       </c>
     </row>
     <row r="133">
@@ -2163,7 +2163,7 @@
         <v>2028</v>
       </c>
       <c r="C133" t="n">
-        <v>157.0412687264329</v>
+        <v>151.9805821906199</v>
       </c>
     </row>
     <row r="134">
@@ -2176,7 +2176,7 @@
         <v>2023</v>
       </c>
       <c r="C134" t="n">
-        <v>1000.071077861472</v>
+        <v>1001.735284150767</v>
       </c>
     </row>
     <row r="135">
@@ -2189,7 +2189,7 @@
         <v>2024</v>
       </c>
       <c r="C135" t="n">
-        <v>1009.986181645835</v>
+        <v>1007.099994460095</v>
       </c>
     </row>
     <row r="136">
@@ -2202,7 +2202,7 @@
         <v>2025</v>
       </c>
       <c r="C136" t="n">
-        <v>1305.641801295834</v>
+        <v>1302.755614110094</v>
       </c>
     </row>
     <row r="137">
@@ -2215,7 +2215,7 @@
         <v>2026</v>
       </c>
       <c r="C137" t="n">
-        <v>1334.243178676604</v>
+        <v>1315.391497500657</v>
       </c>
     </row>
     <row r="138">
@@ -2228,7 +2228,7 @@
         <v>2027</v>
       </c>
       <c r="C138" t="n">
-        <v>1433.394775133789</v>
+        <v>1403.622790975014</v>
       </c>
     </row>
     <row r="139">
@@ -2241,7 +2241,7 @@
         <v>2028</v>
       </c>
       <c r="C139" t="n">
-        <v>1400.829211451735</v>
+        <v>1394.037641173902</v>
       </c>
     </row>
     <row r="140">

</xml_diff>